<commit_message>
Give me a commit!
</commit_message>
<xml_diff>
--- a/planning/Planning 27 Sept/Planning chart.xlsx
+++ b/planning/Planning 27 Sept/Planning chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arjan\Desktop\thesis\thesis\planning\Planning 27 Sept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAF7708B-B99D-4822-9181-500576C90040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CE8729-8D20-4054-BC3E-942CBE45F729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2250" windowWidth="29040" windowHeight="15840" xr2:uid="{7B5F5C66-A64C-4B49-A1A8-63E70B32952D}"/>
   </bookViews>
@@ -418,7 +418,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,12 +441,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -897,14 +891,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515FC7C7-08D1-46ED-8444-D20A2269CEA0}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AJ102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,7 +1149,7 @@
       <c r="V4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:36" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1170,7 +1163,7 @@
       <c r="V5" s="13"/>
       <c r="Z5" s="13"/>
     </row>
-    <row r="6" spans="1:36" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1184,7 +1177,7 @@
       <c r="V6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7" spans="1:36" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1235,7 +1228,7 @@
       <c r="V9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:36" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1249,7 +1242,7 @@
       <c r="V10" s="13"/>
       <c r="Z10" s="13"/>
     </row>
-    <row r="11" spans="1:36" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1263,7 +1256,7 @@
       <c r="V11" s="13"/>
       <c r="Z11" s="13"/>
     </row>
-    <row r="12" spans="1:36" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1294,7 +1287,7 @@
       <c r="V13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:36" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1311,7 +1304,7 @@
       <c r="V14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
-    <row r="15" spans="1:36" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1345,7 +1338,7 @@
       <c r="V16" s="13"/>
       <c r="Z16" s="13"/>
     </row>
-    <row r="17" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1362,7 +1355,7 @@
       <c r="V17" s="13"/>
       <c r="Z17" s="13"/>
     </row>
-    <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1393,7 +1386,7 @@
       <c r="V19" s="13"/>
       <c r="Z19" s="13"/>
     </row>
-    <row r="20" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1407,7 +1400,7 @@
       <c r="V20" s="13"/>
       <c r="Z20" s="13"/>
     </row>
-    <row r="21" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1455,7 +1448,7 @@
       <c r="V23" s="13"/>
       <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
@@ -1469,7 +1462,7 @@
       <c r="V24" s="13"/>
       <c r="Z24" s="13"/>
     </row>
-    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -1483,7 +1476,7 @@
       <c r="V25" s="13"/>
       <c r="Z25" s="13"/>
     </row>
-    <row r="26" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
@@ -1514,7 +1507,7 @@
       <c r="V27" s="13"/>
       <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
@@ -1528,7 +1521,7 @@
       <c r="V28" s="13"/>
       <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>80</v>
       </c>
@@ -1542,7 +1535,7 @@
       <c r="V29" s="13"/>
       <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1556,7 +1549,7 @@
       <c r="V30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>81</v>
       </c>
@@ -1619,7 +1612,7 @@
       <c r="V33" s="13"/>
       <c r="Z33" s="13"/>
     </row>
-    <row r="34" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1633,7 +1626,7 @@
       <c r="V34" s="13"/>
       <c r="Z34" s="13"/>
     </row>
-    <row r="35" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1647,7 +1640,7 @@
       <c r="V35" s="13"/>
       <c r="Z35" s="13"/>
     </row>
-    <row r="36" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -1670,7 +1663,7 @@
       <c r="V36" s="13"/>
       <c r="Z36" s="13"/>
     </row>
-    <row r="37" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -1713,7 +1706,7 @@
       <c r="V38" s="13"/>
       <c r="Z38" s="13"/>
     </row>
-    <row r="39" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -1736,7 +1729,7 @@
       <c r="V39" s="13"/>
       <c r="Z39" s="13"/>
     </row>
-    <row r="40" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
@@ -1753,7 +1746,7 @@
       <c r="V40" s="13"/>
       <c r="Z40" s="13"/>
     </row>
-    <row r="41" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -1770,7 +1763,7 @@
       <c r="V41" s="13"/>
       <c r="Z41" s="13"/>
     </row>
-    <row r="42" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>30</v>
       </c>
@@ -1801,7 +1794,7 @@
       <c r="V43" s="13"/>
       <c r="Z43" s="13"/>
     </row>
-    <row r="44" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -1818,7 +1811,7 @@
       <c r="V44" s="13"/>
       <c r="Z44" s="13"/>
     </row>
-    <row r="45" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -1835,7 +1828,7 @@
       <c r="V45" s="13"/>
       <c r="Z45" s="13"/>
     </row>
-    <row r="46" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
@@ -1852,7 +1845,7 @@
       <c r="V46" s="13"/>
       <c r="Z46" s="13"/>
     </row>
-    <row r="47" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>39</v>
       </c>
@@ -1883,10 +1876,10 @@
         <v>83</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J48" s="10" t="s">
         <v>86</v>
@@ -1912,7 +1905,7 @@
       <c r="V49" s="13"/>
       <c r="Z49" s="13"/>
     </row>
-    <row r="50" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>42</v>
       </c>
@@ -1929,7 +1922,7 @@
       <c r="V50" s="13"/>
       <c r="Z50" s="13"/>
     </row>
-    <row r="51" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>43</v>
       </c>
@@ -1946,7 +1939,7 @@
       <c r="V51" s="13"/>
       <c r="Z51" s="13"/>
     </row>
-    <row r="52" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>44</v>
       </c>
@@ -1980,10 +1973,10 @@
         <v>83</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>86</v>
@@ -1992,7 +1985,7 @@
       <c r="V53" s="13"/>
       <c r="Z53" s="13"/>
     </row>
-    <row r="54" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>46</v>
       </c>
@@ -2009,7 +2002,7 @@
       <c r="V54" s="13"/>
       <c r="Z54" s="13"/>
     </row>
-    <row r="55" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>47</v>
       </c>
@@ -2023,13 +2016,13 @@
         <v>83</v>
       </c>
       <c r="H55" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="U55" s="13"/>
       <c r="V55" s="13"/>
       <c r="Z55" s="13"/>
     </row>
-    <row r="56" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
@@ -2037,10 +2030,10 @@
         <v>3</v>
       </c>
       <c r="H56" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I56" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J56" t="s">
         <v>86</v>
@@ -2049,7 +2042,7 @@
       <c r="V56" s="13"/>
       <c r="Z56" s="13"/>
     </row>
-    <row r="57" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>49</v>
       </c>
@@ -2057,7 +2050,7 @@
         <v>3</v>
       </c>
       <c r="I57" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J57" t="s">
         <v>86</v>
@@ -2088,10 +2081,10 @@
         <v>83</v>
       </c>
       <c r="H59" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I59" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J59" t="s">
         <v>86</v>
@@ -2100,7 +2093,7 @@
       <c r="V59" s="13"/>
       <c r="Z59" s="13"/>
     </row>
-    <row r="60" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>90</v>
       </c>
@@ -2111,16 +2104,16 @@
         <v>83</v>
       </c>
       <c r="H60" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I60" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="U60" s="13"/>
       <c r="V60" s="13"/>
       <c r="Z60" s="13"/>
     </row>
-    <row r="61" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>91</v>
       </c>
@@ -2128,10 +2121,10 @@
         <v>3</v>
       </c>
       <c r="H61" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I61" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J61" t="s">
         <v>86</v>
@@ -2140,7 +2133,7 @@
       <c r="V61" s="13"/>
       <c r="Z61" s="13"/>
     </row>
-    <row r="62" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>92</v>
       </c>
@@ -2148,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="I62" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J62" t="s">
         <v>86</v>
@@ -2157,7 +2150,7 @@
       <c r="V62" s="13"/>
       <c r="Z62" s="13"/>
     </row>
-    <row r="63" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>93</v>
       </c>
@@ -2165,7 +2158,7 @@
         <v>3</v>
       </c>
       <c r="I63" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J63" t="s">
         <v>86</v>
@@ -2174,7 +2167,7 @@
       <c r="V63" s="13"/>
       <c r="Z63" s="13"/>
     </row>
-    <row r="64" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>94</v>
       </c>
@@ -2214,7 +2207,7 @@
       <c r="V65" s="13"/>
       <c r="Z65" s="13"/>
     </row>
-    <row r="66" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>95</v>
       </c>
@@ -2231,7 +2224,7 @@
       <c r="V66" s="13"/>
       <c r="Z66" s="13"/>
     </row>
-    <row r="67" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>96</v>
       </c>
@@ -2254,7 +2247,7 @@
       <c r="V67" s="13"/>
       <c r="Z67" s="13"/>
     </row>
-    <row r="68" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>97</v>
       </c>
@@ -2300,7 +2293,7 @@
       <c r="V69" s="13"/>
       <c r="Z69" s="13"/>
     </row>
-    <row r="70" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>99</v>
       </c>
@@ -2320,7 +2313,7 @@
       <c r="V70" s="13"/>
       <c r="Z70" s="13"/>
     </row>
-    <row r="71" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>100</v>
       </c>
@@ -2340,7 +2333,7 @@
       <c r="V71" s="13"/>
       <c r="Z71" s="13"/>
     </row>
-    <row r="72" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>101</v>
       </c>
@@ -2357,7 +2350,7 @@
       <c r="V72" s="13"/>
       <c r="Z72" s="13"/>
     </row>
-    <row r="73" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>102</v>
       </c>
@@ -2438,7 +2431,7 @@
       </c>
       <c r="Z75" s="13"/>
     </row>
-    <row r="76" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>52</v>
       </c>
@@ -2458,7 +2451,7 @@
       <c r="V76" s="13"/>
       <c r="Z76" s="13"/>
     </row>
-    <row r="77" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>53</v>
       </c>
@@ -2478,7 +2471,7 @@
       <c r="V77" s="13"/>
       <c r="Z77" s="13"/>
     </row>
-    <row r="78" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>54</v>
       </c>
@@ -2498,7 +2491,7 @@
       <c r="V78" s="13"/>
       <c r="Z78" s="13"/>
     </row>
-    <row r="79" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>55</v>
       </c>
@@ -2544,7 +2537,7 @@
       </c>
       <c r="Z80" s="13"/>
     </row>
-    <row r="81" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>57</v>
       </c>
@@ -2564,7 +2557,7 @@
       <c r="V81" s="13"/>
       <c r="Z81" s="13"/>
     </row>
-    <row r="82" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>58</v>
       </c>
@@ -2587,7 +2580,7 @@
       </c>
       <c r="Z82" s="13"/>
     </row>
-    <row r="83" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>59</v>
       </c>
@@ -2615,13 +2608,13 @@
         <v>1</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H84" s="10" t="s">
         <v>86</v>
@@ -2709,10 +2702,10 @@
         <v>83</v>
       </c>
       <c r="F86" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G86" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="U86" s="13"/>
       <c r="V86" s="13"/>
@@ -2729,7 +2722,7 @@
         <v>83</v>
       </c>
       <c r="G87" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H87" t="s">
         <v>86</v>
@@ -2769,7 +2762,7 @@
         <v>2</v>
       </c>
       <c r="H89" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I89" t="s">
         <v>86</v>
@@ -2802,7 +2795,7 @@
       <c r="V89" s="13"/>
       <c r="Z89" s="13"/>
     </row>
-    <row r="90" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>65</v>
       </c>
@@ -2825,7 +2818,7 @@
       <c r="V90" s="13"/>
       <c r="Z90" s="13"/>
     </row>
-    <row r="91" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>66</v>
       </c>
@@ -2854,7 +2847,7 @@
       <c r="V91" s="13"/>
       <c r="Z91" s="13"/>
     </row>
-    <row r="92" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>40</v>
       </c>
@@ -3015,7 +3008,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>71</v>
       </c>
@@ -3029,7 +3022,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="100" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>72</v>
       </c>
@@ -3043,7 +3036,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>73</v>
       </c>
@@ -3057,7 +3050,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:30" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="11" t="s">
         <v>74</v>
       </c>
@@ -3072,15 +3065,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B102" xr:uid="{515FC7C7-08D1-46ED-8444-D20A2269CEA0}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-        <filter val="2"/>
-        <filter val="Level"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:B102" xr:uid="{515FC7C7-08D1-46ED-8444-D20A2269CEA0}"/>
   <conditionalFormatting sqref="C3:AJ102">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="s">
       <formula>NOT(ISERROR(SEARCH("s",C3)))</formula>

</xml_diff>